<commit_message>
Changed file structure some
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Qsync\Graphics I &amp; II Shared Staff Folder\Project &amp; Portfolio IV\Week_3_Handout\Assignments\The Level Renderer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421F74A-5ED2-4C97-92A8-617099FA0AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8EF032-2E9C-4893-867F-354347B73C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="405" windowWidth="28305" windowHeight="16785" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="6255" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1415,6 +1415,9 @@
   </si>
   <si>
     <t>KEY FEATURES - 33% [unlocked by core, pick three]</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -2029,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2044,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -2084,8 +2087,11 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2118,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -2128,8 +2134,11 @@
       <c r="C8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -2140,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -2162,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -2197,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>37</v>
       </c>
@@ -2208,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>36</v>
       </c>

</xml_diff>